<commit_message>
Performed test on an amazon machine
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="59">
   <si>
     <t>Количество строк</t>
   </si>
@@ -156,13 +156,43 @@
     <t>100m</t>
   </si>
   <si>
-    <t>C++</t>
-  </si>
-  <si>
     <t>Postgre</t>
   </si>
   <si>
     <t>sec</t>
+  </si>
+  <si>
+    <t>C++ (my)</t>
+  </si>
+  <si>
+    <t>C++ (amazon)</t>
+  </si>
+  <si>
+    <t>Intel Xeon W3550 3,07Ghz 4 core HP on</t>
+  </si>
+  <si>
+    <t>Threads</t>
+  </si>
+  <si>
+    <t>Processor</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>12 GB</t>
+  </si>
+  <si>
+    <t>vCPUs 16 core</t>
+  </si>
+  <si>
+    <t>64 GB</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -205,13 +235,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -232,13 +271,14 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="2.9284895642962019E-2"/>
-          <c:y val="3.2463507850992307E-2"/>
+          <c:y val="3.2463507850992314E-2"/>
           <c:w val="0.88343995159535038"/>
-          <c:h val="0.89428604319196947"/>
+          <c:h val="0.89428604319196936"/>
         </c:manualLayout>
       </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -248,20 +288,21 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2 C++</c:v>
+                  <c:v>2 C++ (my)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="7"/>
-            <c:spPr>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
-            </c:spPr>
-          </c:marker>
+            </a:ln>
+          </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>Results!$B$3:$B$6</c:f>
@@ -313,20 +354,21 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2 Postgre</c:v>
+                  <c:v>3 C++ (my)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="7"/>
-            <c:spPr>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
               <a:solidFill>
-                <a:srgbClr val="C00000"/>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
-            </c:spPr>
-          </c:marker>
+            </a:ln>
+          </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>Results!$B$3:$B$6</c:f>
@@ -351,19 +393,19 @@
             <c:numRef>
               <c:f>Results!$D$3:$D$6</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>6.0999999999999999E-2</c:v>
+                <c:pt idx="0">
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6</c:v>
+                  <c:v>7.1999999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.9379999999999997</c:v>
+                  <c:v>0.38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.371000000000002</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -378,27 +420,21 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3 C++</c:v>
+                  <c:v>2 C++ (amazon)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln cmpd="dbl">
+            <a:solidFill>
+              <a:srgbClr val="002060"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Results!$B$3:$B$6</c:f>
@@ -426,16 +462,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.5000000000000001E-2</c:v>
+                  <c:v>1.6E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.1999999999999995E-2</c:v>
+                  <c:v>2.1000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.38</c:v>
+                  <c:v>0.11700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3</c:v>
+                  <c:v>1.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -450,27 +486,21 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3 Postgre</c:v>
+                  <c:v>3 C++ (amazon)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7030A0"/>
+            </a:solidFill>
             <a:ln cmpd="dbl">
               <a:solidFill>
-                <a:srgbClr val="C00000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="x"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Results!$B$3:$B$6</c:f>
@@ -495,6 +525,138 @@
             <c:numRef>
               <c:f>Results!$F$3:$F$6</c:f>
               <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Results!$G$1:$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Postgre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:ln cmpd="dbl">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Results!$B$3:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10k</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1m</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10m</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100m</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Results!$G$3:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>6.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.9379999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.371000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Results!$H$1:$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3 Postgre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B0F0"/>
+            </a:solidFill>
+            <a:ln cmpd="dbl">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Results!$B$3:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10k</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1m</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10m</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100m</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Results!$H$3:$H$6</c:f>
+              <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
@@ -513,25 +675,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="57458688"/>
-        <c:axId val="57460224"/>
-      </c:lineChart>
+        <c:axId val="55148544"/>
+        <c:axId val="96918144"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="57458688"/>
+        <c:axId val="55148544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57460224"/>
+        <c:crossAx val="96918144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57460224"/>
+        <c:axId val="96918144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -567,7 +728,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57458688"/>
+        <c:crossAx val="55148544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -582,7 +743,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -598,7 +759,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -908,60 +1069,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" customWidth="1"/>
+    <col min="3" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="C1" s="5">
         <v>2</v>
       </c>
       <c r="D1" s="5">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5">
         <v>2</v>
       </c>
-      <c r="E1" s="5">
-        <v>3</v>
-      </c>
       <c r="F1" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="G1" s="5">
+        <v>2</v>
+      </c>
+      <c r="H1" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:10">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -969,73 +1142,168 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="D3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F3">
+        <v>0.02</v>
+      </c>
+      <c r="G3">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="E3">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F3">
+      <c r="H3">
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:10">
       <c r="B4" t="s">
         <v>43</v>
       </c>
       <c r="C4">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="E4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="F4">
+        <v>3.1E-2</v>
+      </c>
+      <c r="G4" s="2">
         <v>0.6</v>
       </c>
-      <c r="E4">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="H4" s="2">
         <v>0.32500000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="B5" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C5">
         <v>0.5</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
+        <v>0.38</v>
+      </c>
+      <c r="E5">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="G5" s="2">
         <v>5.9379999999999997</v>
       </c>
-      <c r="E5">
-        <v>0.38</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="H5" s="2">
         <v>3.18</v>
       </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C6">
         <v>4.5999999999999996</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
+        <v>3.3</v>
+      </c>
+      <c r="E6">
+        <v>1.02</v>
+      </c>
+      <c r="F6">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="G6" s="2">
         <v>56.371000000000002</v>
       </c>
-      <c r="E6">
-        <v>3.3</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="H6" s="2">
         <v>29.776</v>
       </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="B7" s="1"/>
-      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" t="s">
+        <v>55</v>
+      </c>
+      <c r="G36" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" t="s">
+        <v>57</v>
+      </c>
+      <c r="G37" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" t="s">
+        <v>57</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C36:E36"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>